<commit_message>
add lock screen in step 1 for mitigate mutiples requests
</commit_message>
<xml_diff>
--- a/Listas de precios/mayorista/ARANDELA CHAPISTA y comunes.xlsx
+++ b/Listas de precios/mayorista/ARANDELA CHAPISTA y comunes.xlsx
@@ -904,7 +904,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="n">
-        <v>45344</v>
+        <v>45405</v>
       </c>
       <c r="F1" s="40" t="n"/>
       <c r="G1" s="40" t="n"/>
@@ -1350,37 +1350,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D73:E73"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B52:C52"/>
     <mergeCell ref="D77:E77"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D75:E75"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>